<commit_message>
Validacion Importe Excel y Validacion Practica
</commit_message>
<xml_diff>
--- a/static/files/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/static/files/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\prueva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86C1B60-AB69-4835-A9B1-60E1E092F170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85351120-D6C1-4F44-8E74-7869972F0638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,13 +117,13 @@
     <t>urb. El Ingeniero2</t>
   </si>
   <si>
-    <t>201VP00021</t>
-  </si>
-  <si>
     <t>201VP00022</t>
   </si>
   <si>
-    <t>201VP00027</t>
+    <t>201VP00023</t>
+  </si>
+  <si>
+    <t>201VP00026</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>